<commit_message>
PLA Mk6 and LWPLA Mk7
</commit_message>
<xml_diff>
--- a/LWPLA - Mk7/LWPLA Weights.xlsx
+++ b/LWPLA - Mk7/LWPLA Weights.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hobby\3D Print\Projects\RC\3DPlane\Gaplan\Version7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\Documents\GitHub\Gaplan\LWPLA - Mk7\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -486,7 +486,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>